<commit_message>
set to remove NAs
</commit_message>
<xml_diff>
--- a/DnD_Insults/data/Insults.xlsx
+++ b/DnD_Insults/data/Insults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\OneDrive\Documents\GitHub\shiny-server\DnD_Insults\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="D954AC8449FDB253FADFA499E1ED8189364B648F" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{1B8CA603-C229-49BE-BC0A-1F1347C956F6}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="D954AC8449FDB253FADFA499E1ED8189364B648F" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{F9E1ECC4-6EA3-45EB-86CB-67D0DAB5D692}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="5" xr2:uid="{A6EF34AD-0B09-4017-806A-01A07776BC72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{A6EF34AD-0B09-4017-806A-01A07776BC72}"/>
   </bookViews>
   <sheets>
     <sheet name="Original List" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="172">
   <si>
     <t>What smells worse than a goblin? Oh yeah, you!</t>
   </si>
@@ -449,9 +449,6 @@
     <t>smelt</t>
   </si>
   <si>
-    <t>witnessned</t>
-  </si>
-  <si>
     <t>known</t>
   </si>
   <si>
@@ -546,6 +543,9 @@
   </si>
   <si>
     <t>Punctuation</t>
+  </si>
+  <si>
+    <t>witnessed</t>
   </si>
 </sst>
 </file>
@@ -2782,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864ED301-E378-4FD9-95AA-41B8637D2599}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2799,7 +2799,7 @@
         <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2813,7 +2813,7 @@
         <v>103</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2826,9 +2826,7 @@
       <c r="C3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -2840,9 +2838,7 @@
       <c r="C4" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -2854,51 +2850,43 @@
       <c r="C5" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2913,7 +2901,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2929,7 +2917,7 @@
         <v>131</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2943,7 +2931,7 @@
         <v>132</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2956,9 +2944,7 @@
       <c r="C3" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -2970,9 +2956,7 @@
       <c r="C4" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -2982,11 +2966,9 @@
         <v>127</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>170</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -2996,11 +2978,9 @@
         <v>128</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>170</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -3010,11 +2990,9 @@
         <v>129</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>170</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3028,8 +3006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2D37D4-D013-48C8-B452-FA6B3AEC29E6}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3045,13 +3023,13 @@
         <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3059,13 +3037,13 @@
         <v>136</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3073,13 +3051,13 @@
         <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3087,55 +3065,55 @@
         <v>138</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>